<commit_message>
Having an invalid footprint creates a DQ
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties-2-invalid-footprints.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties-2-invalid-footprints.xlsx
@@ -118,7 +118,7 @@
     <t>Case A-1: 1 Property, 1 Tax Lot</t>
   </si>
   <si>
-    <t>1/5/1888 08:00</t>
+    <t>1/5/17 08:00</t>
   </si>
   <si>
     <t>a</t>
@@ -154,7 +154,7 @@
     <t>d</t>
   </si>
   <si>
-    <t>(( -121.927490629756 37.3966545740305, -121.927428469962 37.3965654556064 ))</t>
+    <t>(( 1 0, 0 1 ))</t>
   </si>
   <si>
     <t>86HJQ8Q5+R6V-1-2-1-1</t>

</xml_diff>